<commit_message>
TIMRLINKN-28 Only try to add project times for existing users
</commit_message>
<xml_diff>
--- a/timrlink.net.CLI.Test/data/projecttime_german_time.xlsx
+++ b/timrlink.net.CLI.Test/data/projecttime_german_time.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sgugarel/Projects/troii/timrlink/timrlink.net/timrlink.net.CLI.Test/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753ECA9D-9E50-C34E-AAF3-8F9E877854F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="9740" yWindow="4440" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="timr" r:id="rId3" sheetId="1"/>
+    <sheet name="timr" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
   <si>
     <t/>
   </si>
@@ -117,22 +125,30 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>John Dow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="dd.MM.yyyy HH:mm"/>
-    <numFmt numFmtId="165" formatCode="dd.MM.yyyy"/>
-    <numFmt numFmtId="166" formatCode="HH:mm"/>
-    <numFmt numFmtId="167" formatCode="[h]:mm"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="dd\.mm\.yyyy"/>
+    <numFmt numFmtId="166" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -143,7 +159,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -158,54 +174,353 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AA4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.0" customWidth="true"/>
-    <col min="2" max="2" width="12.0" customWidth="true"/>
-    <col min="3" max="3" width="24.0" customWidth="true"/>
-    <col min="4" max="4" width="32.0" customWidth="true"/>
-    <col min="5" max="5" width="12.0" customWidth="true"/>
-    <col min="6" max="6" width="18.0" customWidth="true"/>
-    <col min="7" max="7" width="18.0" customWidth="true"/>
-    <col min="8" max="8" width="24.0" customWidth="true"/>
-    <col min="9" max="9" width="10.0" customWidth="true"/>
-    <col min="10" max="10" width="10.0" customWidth="true"/>
-    <col min="11" max="11" width="12.0" customWidth="true"/>
-    <col min="12" max="12" width="10.0" customWidth="true"/>
-    <col min="13" max="13" width="10.0" customWidth="true"/>
-    <col min="14" max="14" width="12.0" customWidth="true"/>
-    <col min="15" max="15" width="10.0" customWidth="true"/>
-    <col min="16" max="16" width="10.0" customWidth="true"/>
-    <col min="17" max="17" width="18.0" customWidth="true"/>
-    <col min="18" max="18" width="18.0" customWidth="true"/>
-    <col min="19" max="19" width="8.0" customWidth="true"/>
-    <col min="20" max="20" width="8.0" customWidth="true"/>
-    <col min="21" max="21" width="12.0" customWidth="true"/>
-    <col min="22" max="22" width="12.0" customWidth="true"/>
-    <col min="23" max="23" width="12.0" customWidth="true"/>
-    <col min="24" max="24" width="18.0" customWidth="true"/>
-    <col min="25" max="25" width="18.0" customWidth="true"/>
-    <col min="26" max="26" width="18.0" customWidth="true"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="32" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
+    <col min="9" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="13" width="10" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="15" max="16" width="10" customWidth="1"/>
+    <col min="17" max="18" width="18" customWidth="1"/>
+    <col min="19" max="20" width="8" customWidth="1"/>
+    <col min="21" max="23" width="12" customWidth="1"/>
+    <col min="24" max="26" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -285,12 +600,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
@@ -310,20 +625,20 @@
       <c r="H2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" t="n" s="2">
-        <v>43585.0</v>
-      </c>
-      <c r="J2" t="n" s="3">
-        <v>43585.63333333333</v>
+      <c r="I2" s="1">
+        <v>43585</v>
+      </c>
+      <c r="J2" s="2">
+        <v>43585.633333333331</v>
       </c>
       <c r="K2" t="s">
         <v>28</v>
       </c>
-      <c r="L2" t="n" s="2">
-        <v>43661.0</v>
-      </c>
-      <c r="M2" t="n" s="3">
-        <v>43661.79861111111</v>
+      <c r="L2" s="1">
+        <v>43661</v>
+      </c>
+      <c r="M2" s="2">
+        <v>43661.798611111109</v>
       </c>
       <c r="N2" t="s">
         <v>28</v>
@@ -340,11 +655,11 @@
       <c r="R2" t="s">
         <v>0</v>
       </c>
-      <c r="S2" t="n" s="4">
-        <v>76.16527791666667</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0.0</v>
+      <c r="S2" s="3">
+        <v>76.165277916666668</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
       </c>
       <c r="U2" t="s">
         <v>0</v>
@@ -359,12 +674,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
-        <v>0</v>
+      <c r="B3" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -375,20 +690,20 @@
       <c r="H3" t="s">
         <v>0</v>
       </c>
-      <c r="I3" t="n" s="2">
-        <v>43585.0</v>
-      </c>
-      <c r="J3" t="n" s="3">
-        <v>43585.63333333333</v>
+      <c r="I3" s="1">
+        <v>43585</v>
+      </c>
+      <c r="J3" s="2">
+        <v>43585.633333333331</v>
       </c>
       <c r="K3" t="s">
         <v>28</v>
       </c>
-      <c r="L3" t="n" s="2">
-        <v>43585.0</v>
-      </c>
-      <c r="M3" t="n" s="3">
-        <v>43585.63333333333</v>
+      <c r="L3" s="1">
+        <v>43585</v>
+      </c>
+      <c r="M3" s="2">
+        <v>43585.633333333331</v>
       </c>
       <c r="N3" t="s">
         <v>28</v>
@@ -405,11 +720,11 @@
       <c r="R3" t="s">
         <v>0</v>
       </c>
-      <c r="S3" t="n" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0.0</v>
+      <c r="S3" s="3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
       </c>
       <c r="U3" t="s">
         <v>0</v>
@@ -427,12 +742,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
-        <v>0</v>
+      <c r="B4" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
@@ -452,20 +767,20 @@
       <c r="H4" t="s">
         <v>0</v>
       </c>
-      <c r="I4" t="n" s="2">
-        <v>43585.0</v>
-      </c>
-      <c r="J4" t="n" s="3">
-        <v>43585.63333333333</v>
+      <c r="I4" s="1">
+        <v>43585</v>
+      </c>
+      <c r="J4" s="2">
+        <v>43585.633333333331</v>
       </c>
       <c r="K4" t="s">
         <v>28</v>
       </c>
-      <c r="L4" t="n" s="2">
-        <v>43585.0</v>
-      </c>
-      <c r="M4" t="n" s="3">
-        <v>43585.63333333333</v>
+      <c r="L4" s="1">
+        <v>43585</v>
+      </c>
+      <c r="M4" s="2">
+        <v>43585.633333333331</v>
       </c>
       <c r="N4" t="s">
         <v>28</v>
@@ -482,11 +797,11 @@
       <c r="R4" t="s">
         <v>0</v>
       </c>
-      <c r="S4" t="n" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="T4" t="n">
-        <v>0.0</v>
+      <c r="S4" s="3">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
       </c>
       <c r="U4" t="s">
         <v>34</v>
@@ -499,6 +814,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>